<commit_message>
Edit some words & final commit
</commit_message>
<xml_diff>
--- a/Week3/Homeworks/Homework6/ABCBank.xlsx
+++ b/Week3/Homeworks/Homework6/ABCBank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gulnu\Desktop\java-camp-2022\Week3\Homeworks\Homework6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A005F2D4-4ECD-41CE-9FE7-FFDA0A1716E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90808B8C-8355-4171-989B-68C776CD3078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="6" xr2:uid="{13625E04-E339-41B5-9E5D-839F4EBE250F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="7" xr2:uid="{13625E04-E339-41B5-9E5D-839F4EBE250F}"/>
   </bookViews>
   <sheets>
     <sheet name="Musteriler" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Bilancolar" sheetId="6" r:id="rId5"/>
     <sheet name="TicariFaaliyetler" sheetId="7" r:id="rId6"/>
     <sheet name="Kanallar" sheetId="8" r:id="rId7"/>
+    <sheet name="Sendikalar" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Id</t>
   </si>
@@ -624,15 +625,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFE08489-6CF8-421A-8FAD-E8637744491B}">
   <dimension ref="A1:B1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D7444F-9ACB-47EB-A69D-74F8939272A2}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>

</xml_diff>